<commit_message>
Post AL test update
Fixed:
- instruction word use : removed congruency, used associate; clarified rating only after 2,5s; adjusted wrap;
-timings: rating does not force ends at encoding. Fixed duration of 2,5s
- key response: only stores one response => data output is not a list
-exemplo_encode.xlsx : fixed object (lure and target) position at 300,xxx
</commit_message>
<xml_diff>
--- a/Exemplo_encode.xlsx
+++ b/Exemplo_encode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vera/Documents/GitHub/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35E9A861-948A-A343-99AB-B5CE8B13DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DF1E60-2523-4841-8E02-6E3FE6DAF27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="7920" windowWidth="20200" windowHeight="5960" xr2:uid="{BC1145FC-44B2-8E4A-B352-2463BCCE776C}"/>
+    <workbookView xWindow="5280" yWindow="7920" windowWidth="22160" windowHeight="8360" xr2:uid="{BC1145FC-44B2-8E4A-B352-2463BCCE776C}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -119,16 +119,16 @@
     <t>target_pos</t>
   </si>
   <si>
-    <t>(250, -200)</t>
-  </si>
-  <si>
-    <t>(250, 200)</t>
-  </si>
-  <si>
     <t>jitter_ITI</t>
   </si>
   <si>
     <t>2.5</t>
+  </si>
+  <si>
+    <t>(300, 200)</t>
+  </si>
+  <si>
+    <t>(300, -200)</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -606,7 +606,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -618,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
@@ -647,7 +647,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
         <v>22</v>
@@ -668,7 +668,7 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>